<commit_message>
fixed various errors, update docs
</commit_message>
<xml_diff>
--- a/src/data/case14.xlsx
+++ b/src/data/case14.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" activeTab="4"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="17040" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
-    <sheet name="generator" sheetId="2" r:id="rId2"/>
-    <sheet name="branch" sheetId="3" r:id="rId3"/>
-    <sheet name="basePower" sheetId="4" r:id="rId4"/>
-    <sheet name="info" sheetId="5" r:id="rId5"/>
+    <sheet name="branch" sheetId="3" r:id="rId2"/>
+    <sheet name="generator" sheetId="2" r:id="rId3"/>
+    <sheet name="generatorcost" sheetId="6" r:id="rId4"/>
+    <sheet name="basePower" sheetId="4" r:id="rId5"/>
+    <sheet name="info" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Bus</t>
   </si>
@@ -247,6 +248,33 @@
   </si>
   <si>
     <t>3 in-service</t>
+  </si>
+  <si>
+    <t>Cost Model</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Piecewise(1), Polynomial(2)</t>
+  </si>
+  <si>
+    <t>Startup [currency]</t>
+  </si>
+  <si>
+    <t>Shutdown [currency]</t>
+  </si>
+  <si>
+    <t>Number of Data Points</t>
+  </si>
+  <si>
+    <t>Coefficient c2</t>
+  </si>
+  <si>
+    <t>Coefficient c1</t>
+  </si>
+  <si>
+    <t>Coefficient c0</t>
   </si>
 </sst>
 </file>
@@ -1282,490 +1310,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U7"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>232.4</v>
-      </c>
-      <c r="C3">
-        <v>-16.899999999999999</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1.06</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>332.4</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>40</v>
-      </c>
-      <c r="C4">
-        <v>42.4</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>-40</v>
-      </c>
-      <c r="F4">
-        <v>1.0449999999999999</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>140</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>23.4</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1.01</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>12.2</v>
-      </c>
-      <c r="D6">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <v>-6</v>
-      </c>
-      <c r="F6">
-        <v>1.07</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>100</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>-6</v>
-      </c>
-      <c r="F7">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>100</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2760,7 +2304,677 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U7"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>232.4</v>
+      </c>
+      <c r="C3">
+        <v>-16.899999999999999</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1.06</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>332.4</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>42.4</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>-40</v>
+      </c>
+      <c r="F4">
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>140</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>23.4</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1.01</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>12.2</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>-6</v>
+      </c>
+      <c r="F6">
+        <v>1.07</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>100</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>-6</v>
+      </c>
+      <c r="F7">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="6" max="7" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4.3029259899999998E-2</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0.25</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -2791,11 +3005,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>